<commit_message>
refresh after NYC and VT trip
</commit_message>
<xml_diff>
--- a/ML_Learning_Buds.xlsx
+++ b/ML_Learning_Buds.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\00_AI.Garden\01_Github\252_ML.tutorial\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\00_TAS\04_Comp.Sci\AI &amp; Machine Learning\Learnings\00_AI.Garden\01_Github\252_ML.tutorial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0CA9051A-3184-4BE1-83D0-7F30A0664607}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD725481-9E7D-489D-B942-8385DD1D98D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="2" xr2:uid="{2AD08176-6702-4455-ABA3-70E607EBFF1E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="7" xr2:uid="{2AD08176-6702-4455-ABA3-70E607EBFF1E}"/>
   </bookViews>
   <sheets>
     <sheet name="Math for ML" sheetId="7" r:id="rId1"/>
@@ -22,19 +22,10 @@
     <sheet name="Reinforcement Learning" sheetId="9" r:id="rId7"/>
     <sheet name="CV apps" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -48,10 +39,19 @@
   <commentList>
     <comment ref="D3" authorId="0" shapeId="0" xr:uid="{033C80A8-2CB3-47AC-986D-29C24E68A1ED}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     github - An introduction and step-by-step implementation</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="175">
   <si>
     <t>Date</t>
   </si>
@@ -554,6 +554,36 @@
   </si>
   <si>
     <t>3. GraphSAGE.ipynb</t>
+  </si>
+  <si>
+    <t>wechat</t>
+  </si>
+  <si>
+    <t>DeepMind學者等《視覺語言預訓練:當前趨勢與未來》教程，闡述最新前沿技術，附Slides (ACL2022)</t>
+  </si>
+  <si>
+    <t>視覺語言概覽 Vision-language landscape before the pretraining era</t>
+  </si>
+  <si>
+    <t>github.io</t>
+  </si>
+  <si>
+    <t>從零開始學習Transformer，手把手寫代碼帶你搞會，11頁pdf細致筆記</t>
+  </si>
+  <si>
+    <t>Transformer-Models-from-Scratch</t>
+  </si>
+  <si>
+    <t>Monash團隊最新《可信圖神經網絡：維度、方法，趨勢》36頁pdf涵蓋闡述可信GNN”六大維度</t>
+  </si>
+  <si>
+    <t>Awesome Resources on Trustworthy Graph Neural Networks</t>
+  </si>
+  <si>
+    <t>Transformers in Vision: From Zero to Hero</t>
+  </si>
+  <si>
+    <t>youtube</t>
   </si>
 </sst>
 </file>
@@ -711,7 +741,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -766,6 +796,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -819,6 +852,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1166,16 +1202,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
@@ -1270,12 +1306,12 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="27" t="s">
         <v>132</v>
       </c>
-      <c r="B9" s="27"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="28"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="29"/>
     </row>
     <row r="10" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A10" s="6">
@@ -1462,16 +1498,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
@@ -1533,10 +1569,10 @@
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="31"/>
-      <c r="B6" s="31"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
+      <c r="A6" s="32"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
     </row>
     <row r="7" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="10"/>
@@ -1575,10 +1611,10 @@
       <c r="D12" s="2"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="30"/>
-      <c r="B13" s="30"/>
-      <c r="C13" s="30"/>
-      <c r="D13" s="30"/>
+      <c r="A13" s="31"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D14" s="2"/>
@@ -1590,10 +1626,10 @@
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" s="30"/>
-      <c r="B17" s="30"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
+      <c r="A17" s="31"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D18" s="2"/>
@@ -1608,10 +1644,10 @@
       <c r="D21" s="2"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" s="30"/>
-      <c r="B22" s="30"/>
-      <c r="C22" s="30"/>
-      <c r="D22" s="30"/>
+      <c r="A22" s="31"/>
+      <c r="B22" s="31"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="31"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D23" s="2"/>
@@ -1620,19 +1656,19 @@
       <c r="D24" s="2"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25" s="30"/>
-      <c r="B25" s="30"/>
-      <c r="C25" s="30"/>
-      <c r="D25" s="30"/>
+      <c r="A25" s="31"/>
+      <c r="B25" s="31"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="31"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D26" s="2"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" s="30"/>
-      <c r="B27" s="30"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="30"/>
+      <c r="A27" s="31"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D28" s="2"/>
@@ -1671,10 +1707,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FACF4494-C8D0-4A92-8B19-C54CAEF52065}">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" outlineLevelRow="1" x14ac:dyDescent="0.35"/>
@@ -1688,16 +1724,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
@@ -1752,11 +1788,11 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
       <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
@@ -2395,6 +2431,22 @@
       </c>
       <c r="E34" s="2" t="s">
         <v>162</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C36" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="D36" s="45" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C37" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -2443,19 +2495,23 @@
     <hyperlink ref="E32" r:id="rId38" display="Graph Attention Networks.ipynb" xr:uid="{233E707F-F680-4968-A5AC-4AB4F8DC08BC}"/>
     <hyperlink ref="E34" r:id="rId39" xr:uid="{07A1ABC3-ADC4-4E84-A869-78AA47BAE2EC}"/>
     <hyperlink ref="E33" r:id="rId40" xr:uid="{4CB89119-93E9-4A72-A0AB-45DEF464B2BB}"/>
+    <hyperlink ref="D36" r:id="rId41" xr:uid="{9FD691DE-3739-4547-8226-8537297FF9A7}"/>
+    <hyperlink ref="C36" r:id="rId42" xr:uid="{49FFF691-33D4-4C96-9F01-0A182F3F3E4A}"/>
+    <hyperlink ref="C37" r:id="rId43" xr:uid="{88966D03-53B8-41A7-9E40-6D2B9C8490C8}"/>
+    <hyperlink ref="D37" r:id="rId44" xr:uid="{4D4C9F5F-FDF0-43F3-9B0D-3B0CA05AD926}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId41"/>
-  <legacyDrawing r:id="rId42"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId45"/>
+  <legacyDrawing r:id="rId46"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BB033FA-4950-4992-A606-6D0F651F64A3}">
-  <dimension ref="A1:H39"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+      <selection activeCell="D44" sqref="C44:D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" outlineLevelRow="1" x14ac:dyDescent="0.35"/>
@@ -2469,16 +2525,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
@@ -2513,7 +2569,7 @@
       <c r="B3" s="4">
         <v>12</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="37" t="s">
         <v>66</v>
       </c>
       <c r="D3" s="7" t="s">
@@ -2536,7 +2592,7 @@
       <c r="B4" s="4">
         <v>12</v>
       </c>
-      <c r="C4" s="37"/>
+      <c r="C4" s="38"/>
       <c r="D4" s="7" t="s">
         <v>64</v>
       </c>
@@ -2600,12 +2656,12 @@
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="38" t="s">
+      <c r="A8" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="39"/>
-      <c r="C8" s="39"/>
-      <c r="D8" s="40"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="41"/>
     </row>
     <row r="9" spans="1:8" s="9" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A9" s="10"/>
@@ -2710,12 +2766,12 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="33" t="s">
+      <c r="A15" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="34"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="35"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="36"/>
     </row>
     <row r="16" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4">
@@ -2769,12 +2825,12 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A19" s="33" t="s">
+      <c r="A19" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="35"/>
+      <c r="B19" s="35"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="36"/>
     </row>
     <row r="20" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4">
@@ -2821,12 +2877,12 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A24" s="33" t="s">
+      <c r="A24" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="B24" s="34"/>
-      <c r="C24" s="34"/>
-      <c r="D24" s="35"/>
+      <c r="B24" s="35"/>
+      <c r="C24" s="35"/>
+      <c r="D24" s="36"/>
     </row>
     <row r="25" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A25" s="4">
@@ -2869,12 +2925,12 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A27" s="33" t="s">
+      <c r="A27" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="B27" s="34"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="35"/>
+      <c r="B27" s="35"/>
+      <c r="C27" s="35"/>
+      <c r="D27" s="36"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="4">
@@ -2897,12 +2953,12 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A29" s="33" t="s">
+      <c r="A29" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="B29" s="34"/>
-      <c r="C29" s="34"/>
-      <c r="D29" s="35"/>
+      <c r="B29" s="35"/>
+      <c r="C29" s="35"/>
+      <c r="D29" s="36"/>
     </row>
     <row r="30" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A30" s="4">
@@ -3024,6 +3080,30 @@
       </c>
       <c r="D39" s="2" t="s">
         <v>139</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C41" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C42" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C44" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -3069,9 +3149,15 @@
     <hyperlink ref="D39" r:id="rId29" location="scrollTo=YRWVLMuqA8jQ" xr:uid="{E13249EA-6346-4FC0-827E-4FDD8BB437CA}"/>
     <hyperlink ref="D7" r:id="rId30" xr:uid="{51DFA512-7B6C-4AB4-BA55-953E49D3E2B1}"/>
     <hyperlink ref="D36" r:id="rId31" xr:uid="{EBDB4986-F757-4F93-9A53-02C39DB6B707}"/>
+    <hyperlink ref="D41" r:id="rId32" xr:uid="{3009E96A-539A-4B86-ADE2-76B0442886C4}"/>
+    <hyperlink ref="C41" r:id="rId33" xr:uid="{C9AE5F27-A3D4-4022-BCD4-794D0BB01950}"/>
+    <hyperlink ref="D42" r:id="rId34" xr:uid="{6B72C2C7-F6DA-4B22-BCE1-07208826420C}"/>
+    <hyperlink ref="C42" r:id="rId35" xr:uid="{FBF4CAF2-9A9B-46BE-81E5-54992A3D78CD}"/>
+    <hyperlink ref="D44" r:id="rId36" xr:uid="{6B8693B6-C445-4590-9C4F-594AAFF51F71}"/>
+    <hyperlink ref="C44" r:id="rId37" xr:uid="{DCC58E05-C78D-4622-B10A-8719B399FDD6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId32"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId38"/>
 </worksheet>
 </file>
 
@@ -3094,16 +3180,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
@@ -3216,10 +3302,10 @@
       <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="30"/>
-      <c r="B12" s="30"/>
-      <c r="C12" s="30"/>
-      <c r="D12" s="30"/>
+      <c r="A12" s="31"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D13" s="2"/>
@@ -3231,10 +3317,10 @@
       <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="30"/>
-      <c r="B16" s="30"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
+      <c r="A16" s="31"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="31"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D17" s="2"/>
@@ -3249,10 +3335,10 @@
       <c r="D20" s="2"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" s="30"/>
-      <c r="B21" s="30"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
+      <c r="A21" s="31"/>
+      <c r="B21" s="31"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D22" s="2"/>
@@ -3261,19 +3347,19 @@
       <c r="D23" s="2"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A24" s="30"/>
-      <c r="B24" s="30"/>
-      <c r="C24" s="30"/>
-      <c r="D24" s="30"/>
+      <c r="A24" s="31"/>
+      <c r="B24" s="31"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="31"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D25" s="2"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" s="30"/>
-      <c r="B26" s="30"/>
-      <c r="C26" s="30"/>
-      <c r="D26" s="30"/>
+      <c r="A26" s="31"/>
+      <c r="B26" s="31"/>
+      <c r="C26" s="31"/>
+      <c r="D26" s="31"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D27" s="2"/>
@@ -3330,16 +3416,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
@@ -3368,12 +3454,12 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="28"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="29"/>
     </row>
     <row r="4" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A4" s="6">
@@ -3638,10 +3724,10 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32" s="30"/>
-      <c r="B32" s="30"/>
-      <c r="C32" s="30"/>
-      <c r="D32" s="30"/>
+      <c r="A32" s="31"/>
+      <c r="B32" s="31"/>
+      <c r="C32" s="31"/>
+      <c r="D32" s="31"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D33" s="2"/>
@@ -3656,10 +3742,10 @@
       <c r="D36" s="2"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A37" s="30"/>
-      <c r="B37" s="30"/>
-      <c r="C37" s="30"/>
-      <c r="D37" s="30"/>
+      <c r="A37" s="31"/>
+      <c r="B37" s="31"/>
+      <c r="C37" s="31"/>
+      <c r="D37" s="31"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D38" s="2"/>
@@ -3668,19 +3754,19 @@
       <c r="D39" s="2"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A40" s="30"/>
-      <c r="B40" s="30"/>
-      <c r="C40" s="30"/>
-      <c r="D40" s="30"/>
+      <c r="A40" s="31"/>
+      <c r="B40" s="31"/>
+      <c r="C40" s="31"/>
+      <c r="D40" s="31"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D41" s="2"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A42" s="30"/>
-      <c r="B42" s="30"/>
-      <c r="C42" s="30"/>
-      <c r="D42" s="30"/>
+      <c r="A42" s="31"/>
+      <c r="B42" s="31"/>
+      <c r="C42" s="31"/>
+      <c r="D42" s="31"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D43" s="2"/>
@@ -3758,16 +3844,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>120</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
@@ -3807,12 +3893,12 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="42" t="s">
         <v>128</v>
       </c>
-      <c r="B4" s="42"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="43"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="44"/>
     </row>
     <row r="5" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A5" s="6">
@@ -3921,10 +4007,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{753D31E3-F8E3-4EE1-927B-A4E92EDB50E0}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3938,16 +4024,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>115</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
@@ -4022,20 +4108,36 @@
     <row r="6" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="15"/>
       <c r="B6" s="15"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="10"/>
+      <c r="C6" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="7" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="15"/>
       <c r="B7" s="15"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
+      <c r="C7" s="26" t="s">
+        <v>168</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="8" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C9" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>173</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4046,8 +4148,14 @@
     <hyperlink ref="D4" r:id="rId2" xr:uid="{22313AA5-1347-4113-91FC-E9700AE59078}"/>
     <hyperlink ref="D5" r:id="rId3" xr:uid="{97695314-7D5E-45B7-9BF3-C3203F9B9F1A}"/>
     <hyperlink ref="C5" r:id="rId4" xr:uid="{54952B4C-0C9F-46A5-AD96-83F9FA003854}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{D8CF873D-D33B-4DCE-A25D-16EDB705B24D}"/>
+    <hyperlink ref="C6" r:id="rId6" xr:uid="{00120FD3-FC0B-459D-A114-D1AFAC32904E}"/>
+    <hyperlink ref="D7" r:id="rId7" xr:uid="{6CBB7A6A-276F-4C51-9060-C63DAF6691BB}"/>
+    <hyperlink ref="C7" r:id="rId8" xr:uid="{C18AEC6D-2815-4348-BCDE-E5ABF3020154}"/>
+    <hyperlink ref="D9" r:id="rId9" xr:uid="{C6D98070-A12E-4515-9E0B-28EE13E9ADC0}"/>
+    <hyperlink ref="C9" r:id="rId10" xr:uid="{DF0946B5-768B-4C4E-A0EA-90838DEB4118}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update GNN and aduio
</commit_message>
<xml_diff>
--- a/ML_Learning_Buds.xlsx
+++ b/ML_Learning_Buds.xlsx
@@ -5,22 +5,23 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\00_TAS\04_Comp.Sci\AI &amp; Machine Learning\Learnings\00_AI.Garden\01_Github\252_ML.tutorial\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\00_AI.Garden\01_Github\252_ML.tutorial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD725481-9E7D-489D-B942-8385DD1D98D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D88D2F0F-0011-4680-AACC-74D1FB3FE218}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="7" xr2:uid="{2AD08176-6702-4455-ABA3-70E607EBFF1E}"/>
+    <workbookView xWindow="-25710" yWindow="-110" windowWidth="25820" windowHeight="13900" tabRatio="605" activeTab="8" xr2:uid="{2AD08176-6702-4455-ABA3-70E607EBFF1E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Math for ML" sheetId="7" r:id="rId1"/>
-    <sheet name="ML adv basics" sheetId="5" r:id="rId2"/>
+    <sheet name="ML.Math" sheetId="7" r:id="rId1"/>
+    <sheet name="ML.Thry" sheetId="5" r:id="rId2"/>
     <sheet name="GNN" sheetId="1" r:id="rId3"/>
     <sheet name="Transformer" sheetId="2" r:id="rId4"/>
-    <sheet name="TransLearning" sheetId="4" r:id="rId5"/>
+    <sheet name="XferLearn" sheetId="4" r:id="rId5"/>
     <sheet name="GAN" sheetId="6" r:id="rId6"/>
-    <sheet name="Reinforcement Learning" sheetId="9" r:id="rId7"/>
-    <sheet name="CV apps" sheetId="8" r:id="rId8"/>
+    <sheet name="RL" sheetId="9" r:id="rId7"/>
+    <sheet name="CV" sheetId="8" r:id="rId8"/>
+    <sheet name="Audio" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,21 +38,12 @@
     <author>tc={033C80A8-2CB3-47AC-986D-29C24E68A1ED}</author>
   </authors>
   <commentList>
-    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{033C80A8-2CB3-47AC-986D-29C24E68A1ED}">
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{033C80A8-2CB3-47AC-986D-29C24E68A1ED}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     github - An introduction and step-by-step implementation</t>
-        </r>
       </text>
     </comment>
   </commentList>
@@ -59,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="204">
   <si>
     <t>Date</t>
   </si>
@@ -584,6 +576,93 @@
   </si>
   <si>
     <t>youtube</t>
+  </si>
+  <si>
+    <t>CNN parameters、FLOPs、MACs、MAC、CIO 計算</t>
+  </si>
+  <si>
+    <t>What Are Graph Neural Networks? How GNNs Work, Explained with Examples</t>
+  </si>
+  <si>
+    <t>Graph Basics and Application</t>
+  </si>
+  <si>
+    <t>Different Graph Neural Network Implementation using PyTorch Geometric</t>
+  </si>
+  <si>
+    <t>Graph Representational Learning</t>
+  </si>
+  <si>
+    <t>graph_neural_network.py</t>
+  </si>
+  <si>
+    <t>Graph Neural Networks: A Deep Neural Network for Graphs</t>
+  </si>
+  <si>
+    <t>Node Classification using Graph Convolutional Neural Network</t>
+  </si>
+  <si>
+    <t>Cora_GCN_medium.ipynb</t>
+  </si>
+  <si>
+    <t>Yolo 2 Explained</t>
+  </si>
+  <si>
+    <t>Towards Geometric Deep Learning I: On the Shoulders of Giants</t>
+  </si>
+  <si>
+    <t>medum</t>
+  </si>
+  <si>
+    <t>A new computational fabric for Graph Neural Networks</t>
+  </si>
+  <si>
+    <t>Building the Vision Transformer From Scratch</t>
+  </si>
+  <si>
+    <t>ViT</t>
+  </si>
+  <si>
+    <t>Stanford CS224W Graph ML Tutorials</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Vision Transfoermer</t>
+  </si>
+  <si>
+    <t>NLP and Audio Applications</t>
+  </si>
+  <si>
+    <t>Releasing Spleeter: Deezer Research source separation engine</t>
+  </si>
+  <si>
+    <t>Source Separation - MIR (Music Information Retrieval)</t>
+  </si>
+  <si>
+    <t>Blind Source Separation in a Nutshell</t>
+  </si>
+  <si>
+    <t>slides</t>
+  </si>
+  <si>
+    <t>github-spleeter</t>
+  </si>
+  <si>
+    <t>Audio Source Separation with Deep Learning</t>
+  </si>
+  <si>
+    <t>website</t>
+  </si>
+  <si>
+    <t>Audio Source Separation on Android with TensorFlow 2.0 (Part I)</t>
+  </si>
+  <si>
+    <t>Audio Source Separation on Android with TensorFlow 2.0 (Part II)</t>
+  </si>
+  <si>
+    <t>Music Source Separation with Spleeter on Google Colab</t>
   </si>
 </sst>
 </file>
@@ -630,7 +709,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -646,6 +725,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -741,7 +826,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -799,6 +884,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -853,8 +947,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1177,7 +1286,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="D3" dT="2022-03-02T15:36:14.69" personId="{8756DFC9-A424-4DD5-90E5-A7E37982BB72}" id="{033C80A8-2CB3-47AC-986D-29C24E68A1ED}">
+  <threadedComment ref="D4" dT="2022-03-02T15:36:14.69" personId="{8756DFC9-A424-4DD5-90E5-A7E37982BB72}" id="{033C80A8-2CB3-47AC-986D-29C24E68A1ED}">
     <text>github - An introduction and step-by-step implementation</text>
   </threadedComment>
 </ThreadedComments>
@@ -1185,10 +1294,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9CF5BD9-6FA7-4FCB-A746-0FAD48EA57C4}">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="A25" sqref="A25:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" outlineLevelRow="1" x14ac:dyDescent="0.35"/>
@@ -1202,16 +1311,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
@@ -1306,12 +1415,12 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="29"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="32"/>
     </row>
     <row r="10" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A10" s="6">
@@ -1446,6 +1555,20 @@
       </c>
       <c r="D23" s="2" t="s">
         <v>149</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" s="6">
+        <v>220708</v>
+      </c>
+      <c r="B25" s="6">
+        <v>7</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -1473,9 +1596,11 @@
     <hyperlink ref="D21" r:id="rId17" xr:uid="{E0108B59-BF75-4DD3-8767-D685824B5901}"/>
     <hyperlink ref="D22" r:id="rId18" xr:uid="{ADB8405B-6981-4F0D-8A35-FF7FBD5FDA48}"/>
     <hyperlink ref="D23" r:id="rId19" xr:uid="{2D94B14E-886F-4838-8714-34F3E8AAD9EB}"/>
+    <hyperlink ref="D25" r:id="rId20" xr:uid="{AE7F79E7-C0A1-4444-8899-EA8F0FBD0F88}"/>
+    <hyperlink ref="C25" r:id="rId21" xr:uid="{C4BC45AA-9A09-4C56-AFC7-1427A1B63DAB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId20"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId22"/>
 </worksheet>
 </file>
 
@@ -1498,16 +1623,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
@@ -1569,10 +1694,10 @@
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="32"/>
-      <c r="B6" s="32"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
+      <c r="A6" s="35"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
     </row>
     <row r="7" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="10"/>
@@ -1611,10 +1736,10 @@
       <c r="D12" s="2"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="31"/>
-      <c r="B13" s="31"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
+      <c r="A13" s="34"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D14" s="2"/>
@@ -1626,10 +1751,10 @@
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" s="31"/>
-      <c r="B17" s="31"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
+      <c r="A17" s="34"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D18" s="2"/>
@@ -1644,10 +1769,10 @@
       <c r="D21" s="2"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" s="31"/>
-      <c r="B22" s="31"/>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31"/>
+      <c r="A22" s="34"/>
+      <c r="B22" s="34"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D23" s="2"/>
@@ -1656,19 +1781,19 @@
       <c r="D24" s="2"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25" s="31"/>
-      <c r="B25" s="31"/>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
+      <c r="A25" s="34"/>
+      <c r="B25" s="34"/>
+      <c r="C25" s="34"/>
+      <c r="D25" s="34"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D26" s="2"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" s="31"/>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
+      <c r="A27" s="34"/>
+      <c r="B27" s="34"/>
+      <c r="C27" s="34"/>
+      <c r="D27" s="34"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D28" s="2"/>
@@ -1707,10 +1832,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FACF4494-C8D0-4A92-8B19-C54CAEF52065}">
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" outlineLevelRow="1" x14ac:dyDescent="0.35"/>
@@ -1724,16 +1849,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
@@ -1762,82 +1887,82 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="16">
+      <c r="A3" s="28">
+        <v>220301</v>
+      </c>
+      <c r="B3" s="28" t="s">
+        <v>191</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="16">
         <v>220219</v>
       </c>
-      <c r="B3" s="16">
-        <v>10</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="17" t="s">
+      <c r="B4" s="16">
+        <v>10</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F4" s="3">
         <v>0.7</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G4" s="3">
         <v>0.6</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H4" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="33" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="2" t="s">
+      <c r="B5" s="36"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="4">
-        <v>220125</v>
-      </c>
-      <c r="B5" s="4">
-        <v>44</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="3">
-        <v>0.95</v>
-      </c>
-      <c r="G5" s="3">
-        <v>0.95</v>
-      </c>
-      <c r="H5" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="4">
-        <v>220204</v>
-      </c>
-      <c r="B6" s="4">
-        <v>6</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>10</v>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="28">
+        <v>220704</v>
+      </c>
+      <c r="B6" s="28">
+        <v>14</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>186</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>14</v>
+        <v>185</v>
       </c>
       <c r="F6" s="3">
-        <v>0.7</v>
+        <v>0.85</v>
       </c>
       <c r="G6" s="3">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="H6" s="3">
         <v>0</v>
@@ -1845,22 +1970,22 @@
     </row>
     <row r="7" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
-        <v>211221</v>
+        <v>220125</v>
       </c>
       <c r="B7" s="4">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F7" s="3">
-        <v>0.8</v>
+        <v>0.95</v>
       </c>
       <c r="G7" s="3">
-        <v>0.9</v>
+        <v>0.95</v>
       </c>
       <c r="H7" s="3">
         <v>0</v>
@@ -1868,22 +1993,22 @@
     </row>
     <row r="8" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
-        <v>211118</v>
+        <v>220204</v>
       </c>
       <c r="B8" s="4">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F8" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="G8" s="3">
         <v>0.8</v>
-      </c>
-      <c r="G8" s="3">
-        <v>0.9</v>
       </c>
       <c r="H8" s="3">
         <v>0</v>
@@ -1891,7 +2016,7 @@
     </row>
     <row r="9" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
-        <v>210619</v>
+        <v>211221</v>
       </c>
       <c r="B9" s="4">
         <v>14</v>
@@ -1900,13 +2025,13 @@
         <v>10</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F9" s="3">
         <v>0.8</v>
       </c>
       <c r="G9" s="3">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="H9" s="3">
         <v>0</v>
@@ -1914,22 +2039,22 @@
     </row>
     <row r="10" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4">
-        <v>210428</v>
+        <v>211118</v>
       </c>
       <c r="B10" s="4">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F10" s="3">
         <v>0.8</v>
       </c>
       <c r="G10" s="3">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="H10" s="3">
         <v>0</v>
@@ -1937,16 +2062,16 @@
     </row>
     <row r="11" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
-        <v>210106</v>
+        <v>210619</v>
       </c>
       <c r="B11" s="4">
+        <v>14</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="F11" s="3">
         <v>0.8</v>
@@ -1959,46 +2084,43 @@
       </c>
     </row>
     <row r="12" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="18">
-        <v>201230</v>
-      </c>
-      <c r="B12" s="18">
-        <v>8</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="19" t="s">
-        <v>118</v>
-      </c>
-      <c r="F12" s="20">
-        <v>0.9</v>
-      </c>
-      <c r="G12" s="20">
+      <c r="A12" s="4">
+        <v>210428</v>
+      </c>
+      <c r="B12" s="4">
+        <v>13</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="3">
         <v>0.8</v>
       </c>
-      <c r="H12" s="20">
-        <v>1</v>
+      <c r="G12" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="H12" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4">
-        <v>200915</v>
+        <v>210106</v>
       </c>
       <c r="B13" s="4">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F13" s="3">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="G13" s="3">
         <v>0.8</v>
@@ -2008,40 +2130,43 @@
       </c>
     </row>
     <row r="14" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="4">
-        <v>200910</v>
-      </c>
-      <c r="B14" s="4">
-        <v>12</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F14" s="3">
+      <c r="A14" s="18">
+        <v>201230</v>
+      </c>
+      <c r="B14" s="18">
+        <v>8</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="F14" s="20">
         <v>0.9</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G14" s="20">
         <v>0.8</v>
       </c>
-      <c r="H14" s="3">
-        <v>0</v>
+      <c r="H14" s="20">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4">
-        <v>200808</v>
+        <v>200915</v>
       </c>
       <c r="B15" s="4">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F15" s="3">
         <v>0.9</v>
@@ -2055,16 +2180,16 @@
     </row>
     <row r="16" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4">
-        <v>200627</v>
+        <v>200910</v>
       </c>
       <c r="B16" s="4">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F16" s="3">
         <v>0.9</v>
@@ -2078,16 +2203,16 @@
     </row>
     <row r="17" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4">
-        <v>200720</v>
+        <v>200808</v>
       </c>
       <c r="B17" s="4">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F17" s="3">
         <v>0.9</v>
@@ -2101,16 +2226,16 @@
     </row>
     <row r="18" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4">
-        <v>200615</v>
+        <v>200627</v>
       </c>
       <c r="B18" s="4">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F18" s="3">
         <v>0.9</v>
@@ -2124,7 +2249,7 @@
     </row>
     <row r="19" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4">
-        <v>200726</v>
+        <v>200720</v>
       </c>
       <c r="B19" s="4">
         <v>9</v>
@@ -2133,7 +2258,7 @@
         <v>10</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F19" s="3">
         <v>0.9</v>
@@ -2145,70 +2270,70 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4">
-        <v>220218</v>
+        <v>200615</v>
       </c>
       <c r="B20" s="4">
+        <v>7</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="G20" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="H20" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="28">
+        <v>220610</v>
+      </c>
+      <c r="B21" s="28">
+        <v>15</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="F21" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="G21" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="H21" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="4">
+        <v>200726</v>
+      </c>
+      <c r="B22" s="4">
         <v>9</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F20" s="3">
-        <v>0.4</v>
-      </c>
-      <c r="G20" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="H20" s="3">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A21" s="4">
-        <v>210526</v>
-      </c>
-      <c r="B21" s="4">
-        <v>6</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F21" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="G21" s="3">
-        <v>0.7</v>
-      </c>
-      <c r="H21" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A22" s="4">
-        <v>210607</v>
-      </c>
-      <c r="B22" s="4">
-        <v>8</v>
-      </c>
       <c r="C22" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F22" s="3">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="G22" s="3">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="H22" s="3">
         <v>0</v>
@@ -2216,45 +2341,45 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="4">
-        <v>210816</v>
+        <v>220218</v>
       </c>
       <c r="B23" s="4">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F23" s="3">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="G23" s="3">
-        <v>0.8</v>
+        <v>0.3</v>
       </c>
       <c r="H23" s="3">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="4">
-        <v>211231</v>
+        <v>210526</v>
       </c>
       <c r="B24" s="4">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F24" s="3">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="G24" s="3">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="H24" s="3">
         <v>0</v>
@@ -2262,22 +2387,22 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="4">
-        <v>220111</v>
+        <v>210607</v>
       </c>
       <c r="B25" s="4">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F25" s="3">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="G25" s="3">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="H25" s="3">
         <v>0</v>
@@ -2285,22 +2410,22 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="4">
-        <v>210621</v>
+        <v>210816</v>
       </c>
       <c r="B26" s="4">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F26" s="3">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="G26" s="3">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="H26" s="3">
         <v>0</v>
@@ -2308,22 +2433,22 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="4">
-        <v>220111</v>
+        <v>211231</v>
       </c>
       <c r="B27" s="4">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F27" s="3">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="G27" s="3">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="H27" s="3">
         <v>0</v>
@@ -2331,22 +2456,22 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="4">
-        <v>181231</v>
+        <v>220111</v>
       </c>
       <c r="B28" s="4">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F28" s="3">
         <v>0.8</v>
       </c>
       <c r="G28" s="3">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="H28" s="3">
         <v>0</v>
@@ -2354,164 +2479,383 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="4">
-        <v>220417</v>
+        <v>210621</v>
       </c>
       <c r="B29" s="4">
-        <v>9</v>
-      </c>
-      <c r="C29" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>154</v>
+        <v>34</v>
+      </c>
+      <c r="F29" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="G29" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="H29" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A30" s="4">
+        <v>220111</v>
+      </c>
+      <c r="B30" s="4">
+        <v>7</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="D30" s="2" t="s">
-        <v>157</v>
+        <v>35</v>
+      </c>
+      <c r="F30" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="G30" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="H30" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" s="4">
+        <v>181231</v>
+      </c>
+      <c r="B31" s="4">
+        <v>9</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F31" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="G31" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="H31" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A32" s="4">
+        <v>220417</v>
+      </c>
+      <c r="B32" s="4">
+        <v>9</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D33" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A34" s="4">
         <v>220220</v>
       </c>
-      <c r="B31" s="4">
+      <c r="B34" s="4">
         <v>30</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C34" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D34" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="E34" s="2" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A32" s="25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A35" s="25">
         <v>220417</v>
       </c>
-      <c r="B32" s="25">
+      <c r="B35" s="25">
         <v>9</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="D35" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="E35" s="2" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" s="25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A36" s="25">
         <v>220421</v>
       </c>
-      <c r="B33" s="25">
+      <c r="B36" s="25">
         <v>9</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D36" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="E36" s="2" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A34" s="4">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A37" s="4">
         <v>220425</v>
       </c>
-      <c r="B34" s="4">
+      <c r="B37" s="4">
         <v>15</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D37" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="E37" s="2" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="C36" s="13" t="s">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C39" s="13" t="s">
         <v>165</v>
       </c>
-      <c r="D36" s="45" t="s">
+      <c r="D39" s="29" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="C37" s="13" t="s">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C40" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D40" s="2" t="s">
         <v>172</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A42" s="4">
+        <v>220201</v>
+      </c>
+      <c r="B42" s="4">
+        <v>16</v>
+      </c>
+      <c r="C42" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="F42" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="G42" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="H42" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C43" s="13"/>
+      <c r="D43" s="2"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A44" s="4">
+        <v>220706</v>
+      </c>
+      <c r="B44" s="4">
+        <v>4</v>
+      </c>
+      <c r="C44" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="F44" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="G44" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="H44" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A45" s="28">
+        <v>220609</v>
+      </c>
+      <c r="B45" s="28">
+        <v>8</v>
+      </c>
+      <c r="C45" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="F45" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="G45" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="H45" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A46" s="4">
+        <v>220614</v>
+      </c>
+      <c r="B46" s="4">
+        <v>8</v>
+      </c>
+      <c r="C46" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="F46" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="G46" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="H46" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A47" s="4">
+        <v>220628</v>
+      </c>
+      <c r="B47" s="4">
+        <v>8</v>
+      </c>
+      <c r="C47" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A48" s="4">
+        <v>220629</v>
+      </c>
+      <c r="B48" s="4">
+        <v>5</v>
+      </c>
+      <c r="C48" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>183</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C5"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" xr:uid="{A41E1DCA-D5EE-4294-A7DB-681E1AB736E1}"/>
-    <hyperlink ref="E3" r:id="rId2" location="scrollTo=8F1Lp6aDKZkT" xr:uid="{05D8E0F1-5FC1-48F4-91B9-50BA36A2E892}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{DE97F4A1-8D65-41D6-BF66-653FC8EDED2B}"/>
-    <hyperlink ref="D5" r:id="rId4" xr:uid="{AC6346A3-0A6E-4D6C-84F6-DBFD338FBEAD}"/>
-    <hyperlink ref="D6" r:id="rId5" xr:uid="{4D68719F-7F51-4345-988C-B1100184014E}"/>
-    <hyperlink ref="D7" r:id="rId6" display="https://medium.com/towards-data-science/using-subgraphs-for-more-expressive-gnns-8d06418d5ab" xr:uid="{651AC25D-90E9-4DF6-B91F-FC3DC64F4C9E}"/>
-    <hyperlink ref="D8" r:id="rId7" display="https://medium.com/towards-data-science/graph-neural-networks-through-the-lens-of-differential-geometry-and-algebraic-topology-3a7c3c22d5f" xr:uid="{0244D791-9D14-401F-AC8F-3966F4CBFCCF}"/>
-    <hyperlink ref="D9" r:id="rId8" display="https://medium.com/towards-data-science/graph-neural-networks-as-neural-diffusion-pdes-8571b8c0c774" xr:uid="{7B1516E8-FE57-4AAC-B42B-95A3881D1AC6}"/>
-    <hyperlink ref="D10" r:id="rId9" display="https://medium.com/towards-data-science/geometric-foundations-of-deep-learning-94cdd45b451d" xr:uid="{F6C68384-8F7F-48D9-AA6A-F6A247972B8B}"/>
-    <hyperlink ref="D11" r:id="rId10" display="https://medium.com/towards-data-science/predictions-and-hopes-for-graph-ml-in-2021-6af2121c3e3d" xr:uid="{D3947BAB-99AE-44B5-A97B-DD7600ADEC4A}"/>
-    <hyperlink ref="D12" r:id="rId11" display="https://medium.com/towards-data-science/geometric-ml-becomes-real-in-fundamental-sciences-3b0d109883b5" xr:uid="{E3456005-3635-4CD0-8FBF-3C641FC9792C}"/>
-    <hyperlink ref="D13" r:id="rId12" display="https://towardsdatascience.com/hyperfoods-9582e5d9a8e4" xr:uid="{287FD61B-E228-48DC-B091-84CE5DBE4604}"/>
-    <hyperlink ref="D14" r:id="rId13" display="https://towardsdatascience.com/manifold-learning-2-99a25eeb677d" xr:uid="{3DF2CB35-1B27-4559-936A-43601F225385}"/>
-    <hyperlink ref="D15" r:id="rId14" display="https://medium.com/towards-data-science/simple-scalable-graph-neural-networks-7eb04f366d07" xr:uid="{3E5EA259-D50E-46FD-967E-CD2BB62143E1}"/>
-    <hyperlink ref="D16" r:id="rId15" display="https://medium.com/towards-data-science/temporal-graph-networks-ab8f327f2efe" xr:uid="{0BCFC289-B748-4F7E-B774-46BB782646E2}"/>
-    <hyperlink ref="D17" r:id="rId16" display="https://towardsdatascience.com/do-we-need-deep-graph-neural-networks-be62d3ec5c59" xr:uid="{84616174-E807-403D-AC06-19CD2A7CD38E}"/>
-    <hyperlink ref="D18" r:id="rId17" display="https://medium.com/towards-data-science/deep-learning-on-graphs-successes-challenges-and-next-steps-7d9ec220ba8" xr:uid="{4ED0B21B-4CA6-4514-8A28-15363FB345F8}"/>
-    <hyperlink ref="D19" r:id="rId18" display="https://towardsdatascience.com/deriving-convolution-from-first-principles-4ff124888028" xr:uid="{039E53ED-DC17-469D-9FBF-84EDF1F18AC5}"/>
-    <hyperlink ref="D20" r:id="rId19" display="https://medium.com/towards-data-science/graph-embeddings-how-nodes-get-mapped-to-vectors-2e12549457ed" xr:uid="{CFEE6A73-7E9D-4F71-AAFD-9DE3F1478F2B}"/>
-    <hyperlink ref="D21" r:id="rId20" display="https://medium.com/towards-data-science/graph-representation-learning-the-encoder-decoder-model-part-2-ed8b505af447" xr:uid="{46671974-2057-4B6B-8574-D0EFB73973AA}"/>
-    <hyperlink ref="D22" r:id="rId21" display="https://medium.com/towards-data-science/node2vec-explained-graphically-749e49b7eb6b" xr:uid="{8BA188F4-A984-447C-8E1A-CECAEFEB98A9}"/>
-    <hyperlink ref="D23" r:id="rId22" display="https://medium.com/towards-data-science/complete-guide-to-understanding-node2vec-algorithm-4e9a35e5d147" xr:uid="{D7AAFB56-9C56-47C1-9FE6-F56E9823CA09}"/>
-    <hyperlink ref="D24" r:id="rId23" display="https://medium.com/@benalex/implement-your-own-music-recommender-with-graph-neural-networks-lightgcn-f59e3bf5f8f5" xr:uid="{CC208B43-8145-4DE3-B3FF-BAF56BEF30BB}"/>
-    <hyperlink ref="D25" r:id="rId24" display="https://medium.com/@pantelis.elinas/scalable-graph-representation-learning-with-graph-neural-networks-a2ab67e06f9" xr:uid="{527CBFC5-2322-4408-8834-87461CD04F79}"/>
-    <hyperlink ref="D26" r:id="rId25" display="https://medium.com/towards-data-science/network-learning-from-network-propagation-to-graph-convolution-eb3c62d09de8" xr:uid="{96A33031-A0BE-4A41-B2FF-3D8958A368D6}"/>
-    <hyperlink ref="D27" r:id="rId26" display="https://medium.com/towards-data-science/knowledge-graph-embedding-a-simplified-version-e6b0a03d373d" xr:uid="{F6DCD3C5-D39B-4AC4-A1E1-107CD326D2CF}"/>
-    <hyperlink ref="D28" r:id="rId27" display="https://medium.com/towards-data-science/graph-embeddings-the-summary-cc6075aba007" xr:uid="{EED9ECA5-23E2-4B60-A0E8-EF7F0C3CC08B}"/>
-    <hyperlink ref="E12" r:id="rId28" xr:uid="{7C3FFD6D-42ED-45F2-B0A7-D6A3C6F2662B}"/>
-    <hyperlink ref="D29" r:id="rId29" xr:uid="{AF533B77-62E1-4CD1-B00C-896036732437}"/>
-    <hyperlink ref="C29" r:id="rId30" xr:uid="{91373D33-B4B1-497D-8E35-449FE3E53F84}"/>
-    <hyperlink ref="E29" r:id="rId31" xr:uid="{3B51ECA3-ADB9-4A2E-ADEF-49EFCAB7D35F}"/>
-    <hyperlink ref="D31" r:id="rId32" display="Introduction to Graph Neural Networks - Graph Convolutional Network in PyTorch" xr:uid="{B8986F82-95C1-4774-A1BD-0833B60C2528}"/>
-    <hyperlink ref="E31" r:id="rId33" xr:uid="{C01C583B-1579-46C1-B4A1-EACCAD582FD2}"/>
-    <hyperlink ref="D30" r:id="rId34" xr:uid="{C2FC7E3F-B049-409F-8EBC-21B18D97A33A}"/>
-    <hyperlink ref="D32" r:id="rId35" xr:uid="{BA025755-C75F-479A-B604-F4EC434350D7}"/>
-    <hyperlink ref="D33" r:id="rId36" xr:uid="{778F81F0-DEB4-4AA4-91FF-DA891FCDC878}"/>
-    <hyperlink ref="D34" r:id="rId37" xr:uid="{A486D461-CD63-46F4-A8BD-875651A27DCE}"/>
-    <hyperlink ref="E32" r:id="rId38" display="Graph Attention Networks.ipynb" xr:uid="{233E707F-F680-4968-A5AC-4AB4F8DC08BC}"/>
-    <hyperlink ref="E34" r:id="rId39" xr:uid="{07A1ABC3-ADC4-4E84-A869-78AA47BAE2EC}"/>
-    <hyperlink ref="E33" r:id="rId40" xr:uid="{4CB89119-93E9-4A72-A0AB-45DEF464B2BB}"/>
-    <hyperlink ref="D36" r:id="rId41" xr:uid="{9FD691DE-3739-4547-8226-8537297FF9A7}"/>
-    <hyperlink ref="C36" r:id="rId42" xr:uid="{49FFF691-33D4-4C96-9F01-0A182F3F3E4A}"/>
-    <hyperlink ref="C37" r:id="rId43" xr:uid="{88966D03-53B8-41A7-9E40-6D2B9C8490C8}"/>
-    <hyperlink ref="D37" r:id="rId44" xr:uid="{4D4C9F5F-FDF0-43F3-9B0D-3B0CA05AD926}"/>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{A41E1DCA-D5EE-4294-A7DB-681E1AB736E1}"/>
+    <hyperlink ref="E4" r:id="rId2" location="scrollTo=8F1Lp6aDKZkT" xr:uid="{05D8E0F1-5FC1-48F4-91B9-50BA36A2E892}"/>
+    <hyperlink ref="D5" r:id="rId3" xr:uid="{DE97F4A1-8D65-41D6-BF66-653FC8EDED2B}"/>
+    <hyperlink ref="D7" r:id="rId4" xr:uid="{AC6346A3-0A6E-4D6C-84F6-DBFD338FBEAD}"/>
+    <hyperlink ref="D8" r:id="rId5" xr:uid="{4D68719F-7F51-4345-988C-B1100184014E}"/>
+    <hyperlink ref="D9" r:id="rId6" display="https://medium.com/towards-data-science/using-subgraphs-for-more-expressive-gnns-8d06418d5ab" xr:uid="{651AC25D-90E9-4DF6-B91F-FC3DC64F4C9E}"/>
+    <hyperlink ref="D10" r:id="rId7" display="https://medium.com/towards-data-science/graph-neural-networks-through-the-lens-of-differential-geometry-and-algebraic-topology-3a7c3c22d5f" xr:uid="{0244D791-9D14-401F-AC8F-3966F4CBFCCF}"/>
+    <hyperlink ref="D11" r:id="rId8" display="https://medium.com/towards-data-science/graph-neural-networks-as-neural-diffusion-pdes-8571b8c0c774" xr:uid="{7B1516E8-FE57-4AAC-B42B-95A3881D1AC6}"/>
+    <hyperlink ref="D12" r:id="rId9" display="https://medium.com/towards-data-science/geometric-foundations-of-deep-learning-94cdd45b451d" xr:uid="{F6C68384-8F7F-48D9-AA6A-F6A247972B8B}"/>
+    <hyperlink ref="D13" r:id="rId10" display="https://medium.com/towards-data-science/predictions-and-hopes-for-graph-ml-in-2021-6af2121c3e3d" xr:uid="{D3947BAB-99AE-44B5-A97B-DD7600ADEC4A}"/>
+    <hyperlink ref="D14" r:id="rId11" display="https://medium.com/towards-data-science/geometric-ml-becomes-real-in-fundamental-sciences-3b0d109883b5" xr:uid="{E3456005-3635-4CD0-8FBF-3C641FC9792C}"/>
+    <hyperlink ref="D15" r:id="rId12" display="https://towardsdatascience.com/hyperfoods-9582e5d9a8e4" xr:uid="{287FD61B-E228-48DC-B091-84CE5DBE4604}"/>
+    <hyperlink ref="D16" r:id="rId13" display="https://towardsdatascience.com/manifold-learning-2-99a25eeb677d" xr:uid="{3DF2CB35-1B27-4559-936A-43601F225385}"/>
+    <hyperlink ref="D17" r:id="rId14" display="https://medium.com/towards-data-science/simple-scalable-graph-neural-networks-7eb04f366d07" xr:uid="{3E5EA259-D50E-46FD-967E-CD2BB62143E1}"/>
+    <hyperlink ref="D18" r:id="rId15" display="https://medium.com/towards-data-science/temporal-graph-networks-ab8f327f2efe" xr:uid="{0BCFC289-B748-4F7E-B774-46BB782646E2}"/>
+    <hyperlink ref="D19" r:id="rId16" display="https://towardsdatascience.com/do-we-need-deep-graph-neural-networks-be62d3ec5c59" xr:uid="{84616174-E807-403D-AC06-19CD2A7CD38E}"/>
+    <hyperlink ref="D20" r:id="rId17" display="https://medium.com/towards-data-science/deep-learning-on-graphs-successes-challenges-and-next-steps-7d9ec220ba8" xr:uid="{4ED0B21B-4CA6-4514-8A28-15363FB345F8}"/>
+    <hyperlink ref="D22" r:id="rId18" display="https://towardsdatascience.com/deriving-convolution-from-first-principles-4ff124888028" xr:uid="{039E53ED-DC17-469D-9FBF-84EDF1F18AC5}"/>
+    <hyperlink ref="D23" r:id="rId19" display="https://medium.com/towards-data-science/graph-embeddings-how-nodes-get-mapped-to-vectors-2e12549457ed" xr:uid="{CFEE6A73-7E9D-4F71-AAFD-9DE3F1478F2B}"/>
+    <hyperlink ref="D24" r:id="rId20" display="https://medium.com/towards-data-science/graph-representation-learning-the-encoder-decoder-model-part-2-ed8b505af447" xr:uid="{46671974-2057-4B6B-8574-D0EFB73973AA}"/>
+    <hyperlink ref="D25" r:id="rId21" display="https://medium.com/towards-data-science/node2vec-explained-graphically-749e49b7eb6b" xr:uid="{8BA188F4-A984-447C-8E1A-CECAEFEB98A9}"/>
+    <hyperlink ref="D26" r:id="rId22" display="https://medium.com/towards-data-science/complete-guide-to-understanding-node2vec-algorithm-4e9a35e5d147" xr:uid="{D7AAFB56-9C56-47C1-9FE6-F56E9823CA09}"/>
+    <hyperlink ref="D27" r:id="rId23" display="https://medium.com/@benalex/implement-your-own-music-recommender-with-graph-neural-networks-lightgcn-f59e3bf5f8f5" xr:uid="{CC208B43-8145-4DE3-B3FF-BAF56BEF30BB}"/>
+    <hyperlink ref="D28" r:id="rId24" display="https://medium.com/@pantelis.elinas/scalable-graph-representation-learning-with-graph-neural-networks-a2ab67e06f9" xr:uid="{527CBFC5-2322-4408-8834-87461CD04F79}"/>
+    <hyperlink ref="D29" r:id="rId25" display="https://medium.com/towards-data-science/network-learning-from-network-propagation-to-graph-convolution-eb3c62d09de8" xr:uid="{96A33031-A0BE-4A41-B2FF-3D8958A368D6}"/>
+    <hyperlink ref="D30" r:id="rId26" display="https://medium.com/towards-data-science/knowledge-graph-embedding-a-simplified-version-e6b0a03d373d" xr:uid="{F6DCD3C5-D39B-4AC4-A1E1-107CD326D2CF}"/>
+    <hyperlink ref="D31" r:id="rId27" display="https://medium.com/towards-data-science/graph-embeddings-the-summary-cc6075aba007" xr:uid="{EED9ECA5-23E2-4B60-A0E8-EF7F0C3CC08B}"/>
+    <hyperlink ref="E14" r:id="rId28" xr:uid="{7C3FFD6D-42ED-45F2-B0A7-D6A3C6F2662B}"/>
+    <hyperlink ref="D32" r:id="rId29" xr:uid="{AF533B77-62E1-4CD1-B00C-896036732437}"/>
+    <hyperlink ref="C32" r:id="rId30" xr:uid="{91373D33-B4B1-497D-8E35-449FE3E53F84}"/>
+    <hyperlink ref="E32" r:id="rId31" xr:uid="{3B51ECA3-ADB9-4A2E-ADEF-49EFCAB7D35F}"/>
+    <hyperlink ref="D34" r:id="rId32" display="Introduction to Graph Neural Networks - Graph Convolutional Network in PyTorch" xr:uid="{B8986F82-95C1-4774-A1BD-0833B60C2528}"/>
+    <hyperlink ref="E34" r:id="rId33" xr:uid="{C01C583B-1579-46C1-B4A1-EACCAD582FD2}"/>
+    <hyperlink ref="D33" r:id="rId34" xr:uid="{C2FC7E3F-B049-409F-8EBC-21B18D97A33A}"/>
+    <hyperlink ref="D35" r:id="rId35" xr:uid="{BA025755-C75F-479A-B604-F4EC434350D7}"/>
+    <hyperlink ref="D36" r:id="rId36" xr:uid="{778F81F0-DEB4-4AA4-91FF-DA891FCDC878}"/>
+    <hyperlink ref="D37" r:id="rId37" xr:uid="{A486D461-CD63-46F4-A8BD-875651A27DCE}"/>
+    <hyperlink ref="E35" r:id="rId38" display="Graph Attention Networks.ipynb" xr:uid="{233E707F-F680-4968-A5AC-4AB4F8DC08BC}"/>
+    <hyperlink ref="E37" r:id="rId39" xr:uid="{07A1ABC3-ADC4-4E84-A869-78AA47BAE2EC}"/>
+    <hyperlink ref="E36" r:id="rId40" xr:uid="{4CB89119-93E9-4A72-A0AB-45DEF464B2BB}"/>
+    <hyperlink ref="D39" r:id="rId41" xr:uid="{9FD691DE-3739-4547-8226-8537297FF9A7}"/>
+    <hyperlink ref="C39" r:id="rId42" xr:uid="{49FFF691-33D4-4C96-9F01-0A182F3F3E4A}"/>
+    <hyperlink ref="C40" r:id="rId43" xr:uid="{88966D03-53B8-41A7-9E40-6D2B9C8490C8}"/>
+    <hyperlink ref="D40" r:id="rId44" xr:uid="{4D4C9F5F-FDF0-43F3-9B0D-3B0CA05AD926}"/>
+    <hyperlink ref="D42" r:id="rId45" xr:uid="{BA535D36-0E74-41C5-8508-1A511335A72D}"/>
+    <hyperlink ref="C42" r:id="rId46" xr:uid="{4685CA28-49D1-4A3F-A218-5CD16868BEC9}"/>
+    <hyperlink ref="D44" r:id="rId47" xr:uid="{328FC9BE-C28B-4EA5-8F64-519FBAB4D896}"/>
+    <hyperlink ref="C44" r:id="rId48" xr:uid="{9CDF84C6-74D1-4CF0-9790-9169964DDBBC}"/>
+    <hyperlink ref="E44" r:id="rId49" xr:uid="{92E25C89-5268-4B8C-AE1C-4AB82B6B03E0}"/>
+    <hyperlink ref="D46" r:id="rId50" xr:uid="{53027B22-841E-4C14-A2E2-B2338924B9D9}"/>
+    <hyperlink ref="C46" r:id="rId51" xr:uid="{A03F1EC2-3E71-46A4-9AEC-A504D2AA0E29}"/>
+    <hyperlink ref="D45" r:id="rId52" xr:uid="{052816F0-EA44-4C89-9633-1F1C3113C5D8}"/>
+    <hyperlink ref="C45" r:id="rId53" xr:uid="{12F480AC-ADF2-49D7-B85B-D5AE852A0679}"/>
+    <hyperlink ref="D47" r:id="rId54" xr:uid="{DAA68FF8-3DFA-4B04-B12F-E256415A7389}"/>
+    <hyperlink ref="C47" r:id="rId55" xr:uid="{CCD58CB5-5889-4876-9FFA-A553751AD063}"/>
+    <hyperlink ref="D48" r:id="rId56" xr:uid="{A1E49AE4-A9E5-49F2-91BB-1742532301A1}"/>
+    <hyperlink ref="C48" r:id="rId57" xr:uid="{AE20511C-09F9-446C-85A3-833DB1C9EB6D}"/>
+    <hyperlink ref="E48" r:id="rId58" xr:uid="{7720EF0A-24DD-434C-8D9D-3B76467B0E12}"/>
+    <hyperlink ref="C6" r:id="rId59" xr:uid="{F13A7CE6-E577-4CA0-B04F-E9932DABD24C}"/>
+    <hyperlink ref="D6" r:id="rId60" xr:uid="{74BB809E-B95C-4A14-885C-E5ADC7135048}"/>
+    <hyperlink ref="C21" r:id="rId61" xr:uid="{B7112CA7-1392-4B5C-9382-DD2A3173C2B2}"/>
+    <hyperlink ref="D21" r:id="rId62" xr:uid="{A75A9F25-F076-45B4-BD67-683A84872367}"/>
+    <hyperlink ref="D3" r:id="rId63" xr:uid="{B722A112-76FE-4063-BBC3-6AF1A825E67D}"/>
+    <hyperlink ref="C3" r:id="rId64" xr:uid="{D167DE14-55D5-4E39-91CA-6A59BC5941D6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId45"/>
-  <legacyDrawing r:id="rId46"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId65"/>
+  <legacyDrawing r:id="rId66"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BB033FA-4950-4992-A606-6D0F651F64A3}">
-  <dimension ref="A1:H44"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D44" sqref="C44:D44"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" outlineLevelRow="1" x14ac:dyDescent="0.35"/>
@@ -2525,16 +2869,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
@@ -2569,7 +2913,7 @@
       <c r="B3" s="4">
         <v>12</v>
       </c>
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="40" t="s">
         <v>66</v>
       </c>
       <c r="D3" s="7" t="s">
@@ -2592,7 +2936,7 @@
       <c r="B4" s="4">
         <v>12</v>
       </c>
-      <c r="C4" s="38"/>
+      <c r="C4" s="41"/>
       <c r="D4" s="7" t="s">
         <v>64</v>
       </c>
@@ -2656,12 +3000,12 @@
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="40"/>
-      <c r="C8" s="40"/>
-      <c r="D8" s="41"/>
+      <c r="B8" s="43"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="44"/>
     </row>
     <row r="9" spans="1:8" s="9" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A9" s="10"/>
@@ -2766,12 +3110,12 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="35"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="36"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="39"/>
     </row>
     <row r="16" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4">
@@ -2825,12 +3169,12 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A19" s="34" t="s">
+      <c r="A19" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="35"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="36"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="39"/>
     </row>
     <row r="20" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4">
@@ -2877,12 +3221,12 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A24" s="34" t="s">
+      <c r="A24" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="B24" s="35"/>
-      <c r="C24" s="35"/>
-      <c r="D24" s="36"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="39"/>
     </row>
     <row r="25" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A25" s="4">
@@ -2904,91 +3248,97 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="4">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26" s="28">
+        <v>220626</v>
+      </c>
+      <c r="B26" s="28">
+        <v>9</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="F26" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="G26" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="H26" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="4">
         <v>220204</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B27" s="4">
         <v>11</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F26" s="3">
+      <c r="F27" s="3">
         <v>0.8</v>
       </c>
-      <c r="G26" s="3">
+      <c r="G27" s="3">
         <v>0.75</v>
       </c>
-      <c r="H26" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A27" s="34" t="s">
+      <c r="H27" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A28" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="B27" s="35"/>
-      <c r="C27" s="35"/>
-      <c r="D27" s="36"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A28" s="4">
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="39"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A29" s="4">
         <v>210723</v>
       </c>
-      <c r="B28" s="4">
-        <v>10</v>
-      </c>
-      <c r="D28" s="1" t="s">
+      <c r="B29" s="4">
+        <v>10</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F28" s="3">
+      <c r="F29" s="3">
         <v>0.5</v>
       </c>
-      <c r="G28" s="3">
+      <c r="G29" s="3">
         <v>0.5</v>
       </c>
-      <c r="H28" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A29" s="34" t="s">
+      <c r="H29" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A30" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="B29" s="35"/>
-      <c r="C29" s="35"/>
-      <c r="D29" s="36"/>
-    </row>
-    <row r="30" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="4">
-        <v>211114</v>
-      </c>
-      <c r="B30" s="4">
-        <v>10</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F30" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="G30" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="H30" s="3">
-        <v>0.6</v>
-      </c>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="39"/>
     </row>
     <row r="31" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A31" s="4">
-        <v>211030</v>
+        <v>211114</v>
       </c>
       <c r="B31" s="4">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F31" s="3">
         <v>0.6</v>
@@ -3008,7 +3358,7 @@
         <v>11</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F32" s="3">
         <v>0.6</v>
@@ -3022,13 +3372,13 @@
     </row>
     <row r="33" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A33" s="4">
-        <v>220127</v>
+        <v>211030</v>
       </c>
       <c r="B33" s="4">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F33" s="3">
         <v>0.6</v>
@@ -3040,77 +3390,97 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="D34" s="2"/>
+    <row r="34" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="4">
+        <v>220127</v>
+      </c>
+      <c r="B34" s="4">
+        <v>5</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F34" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="G34" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="H34" s="3">
+        <v>0.6</v>
+      </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A35" s="4">
+      <c r="D35" s="2"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A36" s="4">
         <v>211113</v>
       </c>
-      <c r="B35" s="4">
+      <c r="B36" s="4">
         <v>9</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D36" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A36" s="21">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A37" s="21">
         <v>210513</v>
       </c>
-      <c r="B36" s="21">
+      <c r="B37" s="21">
         <v>6</v>
       </c>
-      <c r="C36" s="21"/>
-      <c r="D36" s="2" t="s">
+      <c r="C37" s="21"/>
+      <c r="D37" s="2" t="s">
         <v>150</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C38" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C39" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C40" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D40" s="2" t="s">
         <v>139</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C41" s="13" t="s">
-        <v>165</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C42" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C43" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="D43" s="2" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C44" s="13" t="s">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C45" s="13" t="s">
         <v>174</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="D45" s="2" t="s">
         <v>173</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="A24:D24"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A30:D30"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A8:D8"/>
@@ -3127,12 +3497,12 @@
     <hyperlink ref="D22" r:id="rId7" display="https://medium.com/towards-data-science/transformers-explained-visually-part-3-multi-head-attention-deep-dive-1c1ff1024853" xr:uid="{E4F193F9-CB05-46C5-A4C5-558B4F827EA6}"/>
     <hyperlink ref="D23" r:id="rId8" display="https://medium.com/towards-data-science/transformers-explained-visually-not-just-how-but-why-they-work-so-well-d840bd61a9d3" xr:uid="{3BFA1E48-9DC0-4795-B54B-25314DDD03A0}"/>
     <hyperlink ref="D25" r:id="rId9" display="https://medium.com/towards-data-science/understand-and-implement-vision-transformer-with-tensorflow-2-0-f5435769093" xr:uid="{4089316F-52C8-4B16-929A-4B89EE29788D}"/>
-    <hyperlink ref="D26" r:id="rId10" display="https://medium.com/mlearning-ai/vision-transformers-from-scratch-pytorch-a-step-by-step-guide-96c3313c2e0c" xr:uid="{AB9E68DA-96A6-4B2A-9886-442AFE6C85A3}"/>
-    <hyperlink ref="D28" r:id="rId11" display="https://medium.com/towards-data-science/node-embeddings-for-beginners-554ab1625d98" xr:uid="{77B89799-1F5A-4D2D-82C4-7CCBAD79F8EF}"/>
-    <hyperlink ref="D30" r:id="rId12" display="https://medium.com/@naokishibuya/transformers-self-attention-1dc3a2719e0a" xr:uid="{57FC18C8-A328-47D9-91F1-0D4FBBBCAAB4}"/>
-    <hyperlink ref="D31" r:id="rId13" display="https://medium.com/@naokishibuya/positional-encoding-286800cce437" xr:uid="{DA555A6D-778D-477B-AD6F-39C18427B4AE}"/>
-    <hyperlink ref="D32" r:id="rId14" display="https://medium.com/@naokishibuya/transformers-encoder-decoder-434603d19e1" xr:uid="{0FCB5F77-67FC-4995-A8D2-DEDB9E6AE735}"/>
-    <hyperlink ref="D33" r:id="rId15" display="https://medium.com/@monadsblog/multi-head-attention-f2cfb4060e9c" xr:uid="{A6CFB1E4-AB32-436C-AFC5-3754F67DED1C}"/>
+    <hyperlink ref="D27" r:id="rId10" display="https://medium.com/mlearning-ai/vision-transformers-from-scratch-pytorch-a-step-by-step-guide-96c3313c2e0c" xr:uid="{AB9E68DA-96A6-4B2A-9886-442AFE6C85A3}"/>
+    <hyperlink ref="D29" r:id="rId11" display="https://medium.com/towards-data-science/node-embeddings-for-beginners-554ab1625d98" xr:uid="{77B89799-1F5A-4D2D-82C4-7CCBAD79F8EF}"/>
+    <hyperlink ref="D31" r:id="rId12" display="https://medium.com/@naokishibuya/transformers-self-attention-1dc3a2719e0a" xr:uid="{57FC18C8-A328-47D9-91F1-0D4FBBBCAAB4}"/>
+    <hyperlink ref="D32" r:id="rId13" display="https://medium.com/@naokishibuya/positional-encoding-286800cce437" xr:uid="{DA555A6D-778D-477B-AD6F-39C18427B4AE}"/>
+    <hyperlink ref="D33" r:id="rId14" display="https://medium.com/@naokishibuya/transformers-encoder-decoder-434603d19e1" xr:uid="{0FCB5F77-67FC-4995-A8D2-DEDB9E6AE735}"/>
+    <hyperlink ref="D34" r:id="rId15" display="https://medium.com/@monadsblog/multi-head-attention-f2cfb4060e9c" xr:uid="{A6CFB1E4-AB32-436C-AFC5-3754F67DED1C}"/>
     <hyperlink ref="D4" r:id="rId16" xr:uid="{7FFBDC80-D25E-4ED6-9F72-BB08924B7A5A}"/>
     <hyperlink ref="D3" r:id="rId17" xr:uid="{286483FA-4669-476B-8683-B3CCC27AC68C}"/>
     <hyperlink ref="C3:C4" r:id="rId18" display="Pranay Dugar" xr:uid="{9E4C2AB9-5E20-488F-95CF-20B0FE4CECCF}"/>
@@ -3143,21 +3513,24 @@
     <hyperlink ref="A8:D8" r:id="rId23" display="Jay Alammar series" xr:uid="{A6D4A6DC-E86F-4BDB-9B59-3EF9296F2CFE}"/>
     <hyperlink ref="D9" r:id="rId24" xr:uid="{6D0998D3-A750-4483-AEA5-B68C55B576B8}"/>
     <hyperlink ref="D10" r:id="rId25" location="rd" xr:uid="{CCE4EDB6-F198-4062-8FCB-196393994F65}"/>
-    <hyperlink ref="D35" r:id="rId26" xr:uid="{A1FD8657-6A32-4769-AEED-9311E70A2B36}"/>
-    <hyperlink ref="D38" r:id="rId27" xr:uid="{F1EDA837-5B80-4934-9087-223014F5BD44}"/>
+    <hyperlink ref="D36" r:id="rId26" xr:uid="{A1FD8657-6A32-4769-AEED-9311E70A2B36}"/>
+    <hyperlink ref="D39" r:id="rId27" xr:uid="{F1EDA837-5B80-4934-9087-223014F5BD44}"/>
     <hyperlink ref="D6" r:id="rId28" xr:uid="{889F8CAD-E76D-4F6F-8555-37BC41D47A48}"/>
-    <hyperlink ref="D39" r:id="rId29" location="scrollTo=YRWVLMuqA8jQ" xr:uid="{E13249EA-6346-4FC0-827E-4FDD8BB437CA}"/>
+    <hyperlink ref="D40" r:id="rId29" location="scrollTo=YRWVLMuqA8jQ" xr:uid="{E13249EA-6346-4FC0-827E-4FDD8BB437CA}"/>
     <hyperlink ref="D7" r:id="rId30" xr:uid="{51DFA512-7B6C-4AB4-BA55-953E49D3E2B1}"/>
-    <hyperlink ref="D36" r:id="rId31" xr:uid="{EBDB4986-F757-4F93-9A53-02C39DB6B707}"/>
-    <hyperlink ref="D41" r:id="rId32" xr:uid="{3009E96A-539A-4B86-ADE2-76B0442886C4}"/>
-    <hyperlink ref="C41" r:id="rId33" xr:uid="{C9AE5F27-A3D4-4022-BCD4-794D0BB01950}"/>
-    <hyperlink ref="D42" r:id="rId34" xr:uid="{6B72C2C7-F6DA-4B22-BCE1-07208826420C}"/>
-    <hyperlink ref="C42" r:id="rId35" xr:uid="{FBF4CAF2-9A9B-46BE-81E5-54992A3D78CD}"/>
-    <hyperlink ref="D44" r:id="rId36" xr:uid="{6B8693B6-C445-4590-9C4F-594AAFF51F71}"/>
-    <hyperlink ref="C44" r:id="rId37" xr:uid="{DCC58E05-C78D-4622-B10A-8719B399FDD6}"/>
+    <hyperlink ref="D37" r:id="rId31" xr:uid="{EBDB4986-F757-4F93-9A53-02C39DB6B707}"/>
+    <hyperlink ref="D42" r:id="rId32" xr:uid="{3009E96A-539A-4B86-ADE2-76B0442886C4}"/>
+    <hyperlink ref="C42" r:id="rId33" xr:uid="{C9AE5F27-A3D4-4022-BCD4-794D0BB01950}"/>
+    <hyperlink ref="D43" r:id="rId34" xr:uid="{6B72C2C7-F6DA-4B22-BCE1-07208826420C}"/>
+    <hyperlink ref="C43" r:id="rId35" xr:uid="{FBF4CAF2-9A9B-46BE-81E5-54992A3D78CD}"/>
+    <hyperlink ref="D45" r:id="rId36" xr:uid="{6B8693B6-C445-4590-9C4F-594AAFF51F71}"/>
+    <hyperlink ref="C45" r:id="rId37" xr:uid="{DCC58E05-C78D-4622-B10A-8719B399FDD6}"/>
+    <hyperlink ref="D26" r:id="rId38" xr:uid="{8EDC9717-B03D-4CC4-BE1D-9181D4D4C771}"/>
+    <hyperlink ref="C26" r:id="rId39" xr:uid="{8101E90E-81DD-484C-B3A0-4434FFAC7CEB}"/>
+    <hyperlink ref="E26" r:id="rId40" xr:uid="{7967F7FF-1471-4616-8B5B-02E7AC3B87EA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId38"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId41"/>
 </worksheet>
 </file>
 
@@ -3180,16 +3553,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
@@ -3302,10 +3675,10 @@
       <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="31"/>
-      <c r="B12" s="31"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="31"/>
+      <c r="A12" s="34"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D13" s="2"/>
@@ -3317,10 +3690,10 @@
       <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="31"/>
-      <c r="B16" s="31"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
+      <c r="A16" s="34"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D17" s="2"/>
@@ -3335,10 +3708,10 @@
       <c r="D20" s="2"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" s="31"/>
-      <c r="B21" s="31"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
+      <c r="A21" s="34"/>
+      <c r="B21" s="34"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D22" s="2"/>
@@ -3347,19 +3720,19 @@
       <c r="D23" s="2"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A24" s="31"/>
-      <c r="B24" s="31"/>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
+      <c r="A24" s="34"/>
+      <c r="B24" s="34"/>
+      <c r="C24" s="34"/>
+      <c r="D24" s="34"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D25" s="2"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" s="31"/>
-      <c r="B26" s="31"/>
-      <c r="C26" s="31"/>
-      <c r="D26" s="31"/>
+      <c r="A26" s="34"/>
+      <c r="B26" s="34"/>
+      <c r="C26" s="34"/>
+      <c r="D26" s="34"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D27" s="2"/>
@@ -3416,16 +3789,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
@@ -3454,12 +3827,12 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="29"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="32"/>
     </row>
     <row r="4" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A4" s="6">
@@ -3724,10 +4097,10 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32" s="31"/>
-      <c r="B32" s="31"/>
-      <c r="C32" s="31"/>
-      <c r="D32" s="31"/>
+      <c r="A32" s="34"/>
+      <c r="B32" s="34"/>
+      <c r="C32" s="34"/>
+      <c r="D32" s="34"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D33" s="2"/>
@@ -3742,10 +4115,10 @@
       <c r="D36" s="2"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A37" s="31"/>
-      <c r="B37" s="31"/>
-      <c r="C37" s="31"/>
-      <c r="D37" s="31"/>
+      <c r="A37" s="34"/>
+      <c r="B37" s="34"/>
+      <c r="C37" s="34"/>
+      <c r="D37" s="34"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D38" s="2"/>
@@ -3754,19 +4127,19 @@
       <c r="D39" s="2"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A40" s="31"/>
-      <c r="B40" s="31"/>
-      <c r="C40" s="31"/>
-      <c r="D40" s="31"/>
+      <c r="A40" s="34"/>
+      <c r="B40" s="34"/>
+      <c r="C40" s="34"/>
+      <c r="D40" s="34"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D41" s="2"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A42" s="31"/>
-      <c r="B42" s="31"/>
-      <c r="C42" s="31"/>
-      <c r="D42" s="31"/>
+      <c r="A42" s="34"/>
+      <c r="B42" s="34"/>
+      <c r="C42" s="34"/>
+      <c r="D42" s="34"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D43" s="2"/>
@@ -3844,16 +4217,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="33" t="s">
         <v>120</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
@@ -3893,12 +4266,12 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="45" t="s">
         <v>128</v>
       </c>
-      <c r="B4" s="43"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="44"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="47"/>
     </row>
     <row r="5" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A5" s="6">
@@ -4007,13 +4380,13 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{753D31E3-F8E3-4EE1-927B-A4E92EDB50E0}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" outlineLevelRow="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8.7265625" style="6"/>
     <col min="2" max="2" width="6.7265625" style="6" customWidth="1"/>
@@ -4024,16 +4397,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="33" t="s">
         <v>115</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
@@ -4125,23 +4498,91 @@
         <v>167</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="2"/>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="28">
+        <v>220708</v>
+      </c>
+      <c r="B8" s="28">
+        <v>7</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="13"/>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="28"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="6">
+        <v>200607</v>
+      </c>
+      <c r="B12" s="6">
+        <v>6</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="48" t="s">
+        <v>192</v>
+      </c>
+      <c r="B13" s="49"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="50"/>
+    </row>
+    <row r="14" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="6">
+        <v>220626</v>
+      </c>
+      <c r="B14" s="6">
+        <v>9</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="F14" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="G14" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="H14" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="C15" s="13" t="s">
         <v>174</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>173</v>
       </c>
     </row>
+    <row r="16" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35"/>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A13:D13"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E3" r:id="rId1" xr:uid="{02C8AAED-F758-41EE-9E79-A214E9D16DBF}"/>
@@ -4152,10 +4593,227 @@
     <hyperlink ref="C6" r:id="rId6" xr:uid="{00120FD3-FC0B-459D-A114-D1AFAC32904E}"/>
     <hyperlink ref="D7" r:id="rId7" xr:uid="{6CBB7A6A-276F-4C51-9060-C63DAF6691BB}"/>
     <hyperlink ref="C7" r:id="rId8" xr:uid="{C18AEC6D-2815-4348-BCDE-E5ABF3020154}"/>
-    <hyperlink ref="D9" r:id="rId9" xr:uid="{C6D98070-A12E-4515-9E0B-28EE13E9ADC0}"/>
-    <hyperlink ref="C9" r:id="rId10" xr:uid="{DF0946B5-768B-4C4E-A0EA-90838DEB4118}"/>
+    <hyperlink ref="D12" r:id="rId9" xr:uid="{AF4DFF92-31DE-40D0-AF6A-0EF070053FF6}"/>
+    <hyperlink ref="C12" r:id="rId10" xr:uid="{9C72F8A8-D39D-48A3-8E7A-D06E54CB402D}"/>
+    <hyperlink ref="D14" r:id="rId11" xr:uid="{08FA90A5-C734-4CC2-9A8D-2278341C9352}"/>
+    <hyperlink ref="C14" r:id="rId12" xr:uid="{B5A0754C-61FE-4D1F-B8D8-31D8156DA606}"/>
+    <hyperlink ref="E14" r:id="rId13" xr:uid="{36C5277C-E060-4CD0-861D-44B54E58DB55}"/>
+    <hyperlink ref="D15" r:id="rId14" xr:uid="{0B150F92-8E4F-449B-B89E-5C66DEAC4659}"/>
+    <hyperlink ref="C15" r:id="rId15" xr:uid="{342FFFB8-3401-4A19-AEC4-42F7A266D82D}"/>
+    <hyperlink ref="D8" r:id="rId16" xr:uid="{1F775863-8BA8-4368-BF3B-5819A6F82E38}"/>
+    <hyperlink ref="C8" r:id="rId17" xr:uid="{3BF4B091-C94D-4B88-93BB-CD347B31BD6D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId11"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId18"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37BE6095-49DC-40BC-B300-E5D6FBD3C94E}">
+  <dimension ref="A1:H16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" outlineLevelRow="1" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.7265625" style="28"/>
+    <col min="2" max="2" width="6.7265625" style="28" customWidth="1"/>
+    <col min="3" max="3" width="8.7265625" style="28"/>
+    <col min="4" max="4" width="104.7265625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="18.7265625" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="8.7265625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="51" t="s">
+        <v>195</v>
+      </c>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="28">
+        <v>191104</v>
+      </c>
+      <c r="B4" s="28">
+        <v>5</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="28">
+        <v>210428</v>
+      </c>
+      <c r="B5" s="28">
+        <v>9</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="15">
+        <v>200511</v>
+      </c>
+      <c r="B6" s="15">
+        <v>11</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>199</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="15">
+        <v>210113</v>
+      </c>
+      <c r="B7" s="15">
+        <v>7</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="28">
+        <v>210429</v>
+      </c>
+      <c r="B8" s="28">
+        <v>5</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="28">
+        <v>210225</v>
+      </c>
+      <c r="B9" s="28">
+        <v>4</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C11" s="13"/>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C12" s="13"/>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="48"/>
+      <c r="B13" s="49"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="50"/>
+    </row>
+    <row r="14" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="C14" s="13"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="C15" s="13"/>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35"/>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A3:D3"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{19E44AF1-526A-4DB1-A8E7-95D9D913851F}"/>
+    <hyperlink ref="C4" r:id="rId2" xr:uid="{DFA558E1-FB35-408E-A6BA-6EA8F93CD494}"/>
+    <hyperlink ref="E4" r:id="rId3" display="spleeter" xr:uid="{8ED4BA70-AC7B-4BF0-8C66-B4FB3AD1930C}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{04DF5BD4-CCD4-4094-81B2-BC35569C3504}"/>
+    <hyperlink ref="C5" r:id="rId5" xr:uid="{621BB245-2E64-4C13-9679-2DBCAC30B9CE}"/>
+    <hyperlink ref="E5" r:id="rId6" xr:uid="{1741AB3D-7DEE-4D6A-9FDE-EC812ECCE366}"/>
+    <hyperlink ref="D6" r:id="rId7" xr:uid="{4517039E-EEC0-459F-9576-8671FB8FBDBD}"/>
+    <hyperlink ref="C6" r:id="rId8" xr:uid="{B1F32F96-158F-4905-BC06-8B40D5532DFD}"/>
+    <hyperlink ref="E6" r:id="rId9" xr:uid="{D5560C64-BDAB-45B7-8C8F-90F8673BD198}"/>
+    <hyperlink ref="C7" r:id="rId10" xr:uid="{ECFE5EEE-E136-4974-B95D-0EDC03A44E49}"/>
+    <hyperlink ref="D7" r:id="rId11" xr:uid="{A4D2FF90-DB49-4375-AE43-98610FB2DD31}"/>
+    <hyperlink ref="C8" r:id="rId12" xr:uid="{A7B59247-C5AE-434F-B6FC-FEC2D91BF41C}"/>
+    <hyperlink ref="D8" r:id="rId13" xr:uid="{15D8F03F-5B9D-4C59-8BD9-3F3B1BEA2FB2}"/>
+    <hyperlink ref="D9" r:id="rId14" xr:uid="{59313813-AE9F-40F0-91D6-101AE3CE88DE}"/>
+    <hyperlink ref="C9" r:id="rId15" xr:uid="{0CAA5F2C-DE62-4003-AF1F-A89725079D7B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
master table for topics
</commit_message>
<xml_diff>
--- a/ML_Learning_Buds.xlsx
+++ b/ML_Learning_Buds.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\00_AI.Garden\01_Github\252_ML.tutorial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D88D2F0F-0011-4680-AACC-74D1FB3FE218}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{320CEA9E-A5A2-4ABB-BEDD-E8AF223EFD09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25710" yWindow="-110" windowWidth="25820" windowHeight="13900" tabRatio="605" activeTab="8" xr2:uid="{2AD08176-6702-4455-ABA3-70E607EBFF1E}"/>
+    <workbookView xWindow="-25710" yWindow="-110" windowWidth="25820" windowHeight="13900" tabRatio="605" xr2:uid="{2AD08176-6702-4455-ABA3-70E607EBFF1E}"/>
   </bookViews>
   <sheets>
-    <sheet name="ML.Math" sheetId="7" r:id="rId1"/>
-    <sheet name="ML.Thry" sheetId="5" r:id="rId2"/>
-    <sheet name="GNN" sheetId="1" r:id="rId3"/>
-    <sheet name="Transformer" sheetId="2" r:id="rId4"/>
-    <sheet name="XferLearn" sheetId="4" r:id="rId5"/>
-    <sheet name="GAN" sheetId="6" r:id="rId6"/>
-    <sheet name="RL" sheetId="9" r:id="rId7"/>
-    <sheet name="CV" sheetId="8" r:id="rId8"/>
-    <sheet name="Audio" sheetId="10" r:id="rId9"/>
+    <sheet name="MAIN" sheetId="11" r:id="rId1"/>
+    <sheet name="ML.Math" sheetId="7" r:id="rId2"/>
+    <sheet name="ML.Thry" sheetId="5" r:id="rId3"/>
+    <sheet name="GNN" sheetId="1" r:id="rId4"/>
+    <sheet name="Transformer" sheetId="2" r:id="rId5"/>
+    <sheet name="XferLearn" sheetId="4" r:id="rId6"/>
+    <sheet name="GAN" sheetId="6" r:id="rId7"/>
+    <sheet name="RL" sheetId="9" r:id="rId8"/>
+    <sheet name="CV" sheetId="8" r:id="rId9"/>
+    <sheet name="Audio" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -51,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="222">
   <si>
     <t>Date</t>
   </si>
@@ -663,6 +664,60 @@
   </si>
   <si>
     <t>Music Source Separation with Spleeter on Google Colab</t>
+  </si>
+  <si>
+    <t>Master Table For Topics</t>
+  </si>
+  <si>
+    <t>Tab name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>ML.Math</t>
+  </si>
+  <si>
+    <t>Mathematics for Machine Learning</t>
+  </si>
+  <si>
+    <t>MT.thry</t>
+  </si>
+  <si>
+    <t>Basic Concentps and Advanced Topics/Theories for  Machine Learning</t>
+  </si>
+  <si>
+    <t>GNN</t>
+  </si>
+  <si>
+    <t>Graph Neural Netowrks</t>
+  </si>
+  <si>
+    <t>Transformer theories and Applications in NLP and Vision Applications</t>
+  </si>
+  <si>
+    <t>XferLearn</t>
+  </si>
+  <si>
+    <t>Transfer Learning</t>
+  </si>
+  <si>
+    <t>GAN</t>
+  </si>
+  <si>
+    <t>Gererative Adversarial Learning (GAN)</t>
+  </si>
+  <si>
+    <t>RL</t>
+  </si>
+  <si>
+    <t>CV</t>
+  </si>
+  <si>
+    <t>Computer Vision Applications</t>
+  </si>
+  <si>
+    <t>Audio</t>
   </si>
 </sst>
 </file>
@@ -826,7 +881,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -964,6 +1019,27 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1293,6 +1369,404 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45C27551-AED4-426B-A61B-92F0AB61574A}">
+  <dimension ref="A1:H15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" outlineLevelRow="1" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.7265625" style="28"/>
+    <col min="2" max="2" width="6.7265625" style="28" customWidth="1"/>
+    <col min="3" max="3" width="8.7265625" style="28"/>
+    <col min="4" max="4" width="59.81640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="18.7265625" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="8.7265625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="60" t="s">
+        <v>204</v>
+      </c>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="54" t="s">
+        <v>205</v>
+      </c>
+      <c r="B2" s="55"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="3" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="57" t="s">
+        <v>207</v>
+      </c>
+      <c r="B3" s="58"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="2" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="57" t="s">
+        <v>209</v>
+      </c>
+      <c r="B4" s="58"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="2" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="57" t="s">
+        <v>211</v>
+      </c>
+      <c r="B5" s="58"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="57" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="58"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="57" t="s">
+        <v>214</v>
+      </c>
+      <c r="B7" s="58"/>
+      <c r="C7" s="59"/>
+      <c r="D7" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="57" t="s">
+        <v>216</v>
+      </c>
+      <c r="B8" s="58"/>
+      <c r="C8" s="59"/>
+      <c r="D8" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="57" t="s">
+        <v>218</v>
+      </c>
+      <c r="B9" s="58"/>
+      <c r="C9" s="59"/>
+      <c r="D9" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="57" t="s">
+        <v>219</v>
+      </c>
+      <c r="B10" s="58"/>
+      <c r="C10" s="59"/>
+      <c r="D10" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="57" t="s">
+        <v>221</v>
+      </c>
+      <c r="B11" s="58"/>
+      <c r="C11" s="59"/>
+      <c r="D11" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="54"/>
+      <c r="B12" s="55"/>
+      <c r="C12" s="56"/>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="54"/>
+      <c r="B13" s="55"/>
+      <c r="C13" s="56"/>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="54"/>
+      <c r="B14" s="55"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" s="54"/>
+      <c r="B15" s="55"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A3:C3" location="ML.Math!A1" display="ML.Math" xr:uid="{4B3F88EE-FD09-4CD6-9621-B148374D0001}"/>
+    <hyperlink ref="A4:C4" location="ML.Thry!A1" display="MT.thry" xr:uid="{8735481F-FC9C-43BE-B7C6-A2663E5E5576}"/>
+    <hyperlink ref="A5:C5" location="GNN!A1" display="GNN" xr:uid="{B8CC83DB-FCE7-4A5B-86ED-938679BDC3E5}"/>
+    <hyperlink ref="A6:C6" location="Transformer!A1" display="Transformer" xr:uid="{5DBADD02-4DDE-49B6-95EB-B12EE1DBC69F}"/>
+    <hyperlink ref="A7:C7" location="XferLearn!A1" display="XferLearn" xr:uid="{FF6ACBC8-479C-486A-89F5-49418CB0A0FD}"/>
+    <hyperlink ref="A8:C8" location="GAN!A1" display="GAN" xr:uid="{EC521432-416A-4908-9B90-9D8A76CA5311}"/>
+    <hyperlink ref="A9:C9" location="RL!A1" display="RL" xr:uid="{19A90A58-A770-4E9C-9E66-658EA484B62A}"/>
+    <hyperlink ref="A10:C10" location="CV!A1" display="CV" xr:uid="{7DD87C23-FBF2-4822-9C53-60DCE84080BD}"/>
+    <hyperlink ref="A11:C11" location="Audio!A1" display="Audio" xr:uid="{4BE67B89-66F5-4A6F-8E21-BDF9E383276A}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37BE6095-49DC-40BC-B300-E5D6FBD3C94E}">
+  <dimension ref="A1:H16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" outlineLevelRow="1" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.7265625" style="28"/>
+    <col min="2" max="2" width="6.7265625" style="28" customWidth="1"/>
+    <col min="3" max="3" width="8.7265625" style="28"/>
+    <col min="4" max="4" width="104.7265625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="18.7265625" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="8.7265625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="51" t="s">
+        <v>195</v>
+      </c>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="28">
+        <v>191104</v>
+      </c>
+      <c r="B4" s="28">
+        <v>5</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="28">
+        <v>210428</v>
+      </c>
+      <c r="B5" s="28">
+        <v>9</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="15">
+        <v>200511</v>
+      </c>
+      <c r="B6" s="15">
+        <v>11</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>199</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="15">
+        <v>210113</v>
+      </c>
+      <c r="B7" s="15">
+        <v>7</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="28">
+        <v>210429</v>
+      </c>
+      <c r="B8" s="28">
+        <v>5</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="28">
+        <v>210225</v>
+      </c>
+      <c r="B9" s="28">
+        <v>4</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C11" s="13"/>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C12" s="13"/>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="48"/>
+      <c r="B13" s="49"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="50"/>
+    </row>
+    <row r="14" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="C14" s="13"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="C15" s="13"/>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35"/>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A3:D3"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{19E44AF1-526A-4DB1-A8E7-95D9D913851F}"/>
+    <hyperlink ref="C4" r:id="rId2" xr:uid="{DFA558E1-FB35-408E-A6BA-6EA8F93CD494}"/>
+    <hyperlink ref="E4" r:id="rId3" display="spleeter" xr:uid="{8ED4BA70-AC7B-4BF0-8C66-B4FB3AD1930C}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{04DF5BD4-CCD4-4094-81B2-BC35569C3504}"/>
+    <hyperlink ref="C5" r:id="rId5" xr:uid="{621BB245-2E64-4C13-9679-2DBCAC30B9CE}"/>
+    <hyperlink ref="E5" r:id="rId6" xr:uid="{1741AB3D-7DEE-4D6A-9FDE-EC812ECCE366}"/>
+    <hyperlink ref="D6" r:id="rId7" xr:uid="{4517039E-EEC0-459F-9576-8671FB8FBDBD}"/>
+    <hyperlink ref="C6" r:id="rId8" xr:uid="{B1F32F96-158F-4905-BC06-8B40D5532DFD}"/>
+    <hyperlink ref="E6" r:id="rId9" xr:uid="{D5560C64-BDAB-45B7-8C8F-90F8673BD198}"/>
+    <hyperlink ref="C7" r:id="rId10" xr:uid="{ECFE5EEE-E136-4974-B95D-0EDC03A44E49}"/>
+    <hyperlink ref="D7" r:id="rId11" xr:uid="{A4D2FF90-DB49-4375-AE43-98610FB2DD31}"/>
+    <hyperlink ref="C8" r:id="rId12" xr:uid="{A7B59247-C5AE-434F-B6FC-FEC2D91BF41C}"/>
+    <hyperlink ref="D8" r:id="rId13" xr:uid="{15D8F03F-5B9D-4C59-8BD9-3F3B1BEA2FB2}"/>
+    <hyperlink ref="D9" r:id="rId14" xr:uid="{59313813-AE9F-40F0-91D6-101AE3CE88DE}"/>
+    <hyperlink ref="C9" r:id="rId15" xr:uid="{0CAA5F2C-DE62-4003-AF1F-A89725079D7B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId16"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9CF5BD9-6FA7-4FCB-A746-0FAD48EA57C4}">
   <dimension ref="A1:H25"/>
   <sheetViews>
@@ -1604,7 +2078,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBDA65ED-4C85-4861-82CF-F291D7C6B4B4}">
   <dimension ref="A1:H32"/>
   <sheetViews>
@@ -1830,7 +2304,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FACF4494-C8D0-4A92-8B19-C54CAEF52065}">
   <dimension ref="A1:H48"/>
   <sheetViews>
@@ -2850,7 +3324,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BB033FA-4950-4992-A606-6D0F651F64A3}">
   <dimension ref="A1:H45"/>
   <sheetViews>
@@ -3534,7 +4008,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{973EC531-5798-435B-8029-F6E0E96262FE}">
   <dimension ref="A1:H31"/>
   <sheetViews>
@@ -3770,7 +4244,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D16140C-1AD4-48A6-965C-4CB846C9F250}">
   <dimension ref="A1:H47"/>
   <sheetViews>
@@ -4198,7 +4672,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BCDE4AC-D7A7-4446-A810-10F8E7FDFAFC}">
   <dimension ref="A1:H10"/>
   <sheetViews>
@@ -4378,7 +4852,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{753D31E3-F8E3-4EE1-927B-A4E92EDB50E0}">
   <dimension ref="A1:H16"/>
   <sheetViews>
@@ -4606,214 +5080,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId18"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37BE6095-49DC-40BC-B300-E5D6FBD3C94E}">
-  <dimension ref="A1:H16"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" outlineLevelRow="1" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="8.7265625" style="28"/>
-    <col min="2" max="2" width="6.7265625" style="28" customWidth="1"/>
-    <col min="3" max="3" width="8.7265625" style="28"/>
-    <col min="4" max="4" width="104.7265625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="18.7265625" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="3"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="33" t="s">
-        <v>193</v>
-      </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="51" t="s">
-        <v>195</v>
-      </c>
-      <c r="B3" s="52"/>
-      <c r="C3" s="52"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="28">
-        <v>191104</v>
-      </c>
-      <c r="B4" s="28">
-        <v>5</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="28">
-        <v>210428</v>
-      </c>
-      <c r="B5" s="28">
-        <v>9</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="15">
-        <v>200511</v>
-      </c>
-      <c r="B6" s="15">
-        <v>11</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="D6" s="27" t="s">
-        <v>199</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="15">
-        <v>210113</v>
-      </c>
-      <c r="B7" s="15">
-        <v>7</v>
-      </c>
-      <c r="C7" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="27" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="28">
-        <v>210429</v>
-      </c>
-      <c r="B8" s="28">
-        <v>5</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="28">
-        <v>210225</v>
-      </c>
-      <c r="B9" s="28">
-        <v>4</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C11" s="13"/>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C12" s="13"/>
-      <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="48"/>
-      <c r="B13" s="49"/>
-      <c r="C13" s="49"/>
-      <c r="D13" s="50"/>
-    </row>
-    <row r="14" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="C14" s="13"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="C15" s="13"/>
-      <c r="D15" s="2"/>
-    </row>
-    <row r="16" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.35"/>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="A3:D3"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="D4" r:id="rId1" xr:uid="{19E44AF1-526A-4DB1-A8E7-95D9D913851F}"/>
-    <hyperlink ref="C4" r:id="rId2" xr:uid="{DFA558E1-FB35-408E-A6BA-6EA8F93CD494}"/>
-    <hyperlink ref="E4" r:id="rId3" display="spleeter" xr:uid="{8ED4BA70-AC7B-4BF0-8C66-B4FB3AD1930C}"/>
-    <hyperlink ref="D5" r:id="rId4" xr:uid="{04DF5BD4-CCD4-4094-81B2-BC35569C3504}"/>
-    <hyperlink ref="C5" r:id="rId5" xr:uid="{621BB245-2E64-4C13-9679-2DBCAC30B9CE}"/>
-    <hyperlink ref="E5" r:id="rId6" xr:uid="{1741AB3D-7DEE-4D6A-9FDE-EC812ECCE366}"/>
-    <hyperlink ref="D6" r:id="rId7" xr:uid="{4517039E-EEC0-459F-9576-8671FB8FBDBD}"/>
-    <hyperlink ref="C6" r:id="rId8" xr:uid="{B1F32F96-158F-4905-BC06-8B40D5532DFD}"/>
-    <hyperlink ref="E6" r:id="rId9" xr:uid="{D5560C64-BDAB-45B7-8C8F-90F8673BD198}"/>
-    <hyperlink ref="C7" r:id="rId10" xr:uid="{ECFE5EEE-E136-4974-B95D-0EDC03A44E49}"/>
-    <hyperlink ref="D7" r:id="rId11" xr:uid="{A4D2FF90-DB49-4375-AE43-98610FB2DD31}"/>
-    <hyperlink ref="C8" r:id="rId12" xr:uid="{A7B59247-C5AE-434F-B6FC-FEC2D91BF41C}"/>
-    <hyperlink ref="D8" r:id="rId13" xr:uid="{15D8F03F-5B9D-4C59-8BD9-3F3B1BEA2FB2}"/>
-    <hyperlink ref="D9" r:id="rId14" xr:uid="{59313813-AE9F-40F0-91D6-101AE3CE88DE}"/>
-    <hyperlink ref="C9" r:id="rId15" xr:uid="{0CAA5F2C-DE62-4003-AF1F-A89725079D7B}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId16"/>
-</worksheet>
 </file>
</xml_diff>